<commit_message>
RPA-100: Har lagt utkast for input excel fil for del 4
</commit_message>
<xml_diff>
--- a/Vasklister/Excel/vaskeliste_saknr.xlsx
+++ b/Vasklister/Excel/vaskeliste_saknr.xlsx
@@ -11,41 +11,17 @@
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>debitor_ident</t>
   </si>
   <si>
     <t>Sak_Nr</t>
-  </si>
-  <si>
-    <t>02037622764</t>
-  </si>
-  <si>
-    <t>02058143173</t>
-  </si>
-  <si>
-    <t>02065143855</t>
-  </si>
-  <si>
-    <t>02068925943</t>
-  </si>
-  <si>
-    <t>02088731266</t>
-  </si>
-  <si>
-    <t>02098931107</t>
-  </si>
-  <si>
-    <t>02116945668</t>
-  </si>
-  <si>
-    <t>03017047700</t>
   </si>
 </sst>
 </file>
@@ -69,7 +45,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,16 +53,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,68 +401,40 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>119467</v>
+      <c r="A2" s="3">
+        <v>13088334935</v>
+      </c>
+      <c r="B2" s="3">
+        <v>267794</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>252487</v>
+      <c r="A3" s="3">
+        <v>13098245418</v>
+      </c>
+      <c r="B3" s="3">
+        <v>313054</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>203247</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>244562</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>299970</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>299870</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>260678</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1">
-        <v>237349</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>